<commit_message>
Added time worked for Kevin
</commit_message>
<xml_diff>
--- a/TI_Senior_Time_Tracking.xlsx
+++ b/TI_Senior_Time_Tracking.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\K_Documents\CEN4908C\Senior_Design_TI_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C83176A9-FB79-4872-AE84-B54D17876827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D2EBE7-FC1A-415A-8D29-38698A1744C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{CC5CD12B-A517-4AD2-8F94-0FCB461D9F37}"/>
+    <workbookView xWindow="2620" yWindow="2620" windowWidth="14400" windowHeight="8170" xr2:uid="{CC5CD12B-A517-4AD2-8F94-0FCB461D9F37}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="81">
   <si>
     <t>Tasks</t>
   </si>
@@ -276,6 +276,9 @@
   </si>
   <si>
     <t>Researched and created schematic for USB connector and voltage suppressor.</t>
+  </si>
+  <si>
+    <t>Worked on mmWave Radar PCB schematic. Work included drawing components and connecting components.</t>
   </si>
 </sst>
 </file>
@@ -794,8 +797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4279954-09A6-4900-9B97-A5C01497F037}">
   <dimension ref="A1:G76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="G83" sqref="G83"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="I76" sqref="I76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2326,13 +2329,25 @@
         <v>79</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B76" s="13"/>
-      <c r="C76" s="14"/>
-      <c r="D76" s="15"/>
-      <c r="E76" s="15"/>
-      <c r="F76" s="16"/>
-      <c r="G76" s="13"/>
+    <row r="76" spans="1:7" ht="189" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B76" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C76" s="14">
+        <v>45676</v>
+      </c>
+      <c r="D76" s="15">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E76" s="15">
+        <v>0.6875</v>
+      </c>
+      <c r="F76" s="16">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="G76" s="13" t="s">
+        <v>80</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2340,6 +2355,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EEE4306558685A49A8565CD439201237" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5064c96a065c23450bae9488bc93af03">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5ad209e5-25fd-49ac-a194-a52849a11728" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e40702559d6d17f3ed5d7744699d9b14" ns3:_="">
     <xsd:import namespace="5ad209e5-25fd-49ac-a194-a52849a11728"/>
@@ -2495,15 +2519,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2513,6 +2528,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FAA5AE56-6ED0-42AD-90B5-C3A656DA6CBB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8ECEEE9E-3EE2-4A26-BE08-0E4EE09F3232}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2526,14 +2549,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FAA5AE56-6ED0-42AD-90B5-C3A656DA6CBB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>